<commit_message>
Feature: new function: Write to baseworkspace
</commit_message>
<xml_diff>
--- a/matCompareSrcCode/UI/Common/Text/TextData.xlsx
+++ b/matCompareSrcCode/UI/Common/Text/TextData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramFiles\MatlabProjects\matCompare\matCompareSrcCode\UI\Common\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1573401-8C62-4D60-8B92-19F93D5D1441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF6BF8-990B-4F1F-A5CE-CBAFBB2F1D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50" yWindow="20" windowWidth="25550" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="148">
   <si>
     <t>Chinese</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -504,6 +504,18 @@
   </si>
   <si>
     <t>By visdiff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write result to BaseWorkSpace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并结果写到基础工作区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>マージ結果をベースワークスペースに書き込む</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA45CA80-1BF4-4511-9958-95D8EE1C2744}" name="表1" displayName="表1" ref="A1:E38" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:E38" xr:uid="{FA45CA80-1BF4-4511-9958-95D8EE1C2744}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA45CA80-1BF4-4511-9958-95D8EE1C2744}" name="表1" displayName="表1" ref="A1:E39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:E39" xr:uid="{FA45CA80-1BF4-4511-9958-95D8EE1C2744}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E72057ED-C2A8-4E05-849C-9FF930CCAFC7}" name="IndexNum"/>
     <tableColumn id="2" xr3:uid="{9B261824-20EF-4604-A69C-D58BB222F516}" name="IndexStr"/>
@@ -946,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1607,6 +1619,23 @@
         <v>142</v>
       </c>
     </row>
+    <row r="39" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>